<commit_message>
remove blank text nodes
</commit_message>
<xml_diff>
--- a/mwConfigParser_result_20180602.xlsx
+++ b/mwConfigParser_result_20180602.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="15">
   <si>
     <t>Item</t>
   </si>
@@ -54,12 +54,6 @@
   </si>
   <si>
     <t>null</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;Host appBase="webapps" autoDeploy="true" name="localhost" unpackWARs="true"&gt;
-        &lt;Valve className="org.apache.catalina.valves.AccessLogValve" directory="logs" pattern="%h %l %u %t &amp;quot;%r&amp;quot; %s %b" prefix="localhost_access_log" suffix=".txt"/&gt;
-      &lt;/Host&gt;
-</t>
   </si>
   <si>
     <t>default(not use)(context.xml)
@@ -314,7 +308,7 @@
         <v>7</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C13"/>
       <c r="D13"/>
@@ -326,7 +320,7 @@
         <v>8</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C14"/>
       <c r="D14"/>

</xml_diff>

<commit_message>
remove black text node
</commit_message>
<xml_diff>
--- a/mwConfigParser_result_20180602.xlsx
+++ b/mwConfigParser_result_20180602.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="16">
   <si>
     <t>Item</t>
   </si>
@@ -54,6 +54,12 @@
   </si>
   <si>
     <t>null</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;Host appBase="webapps" autoDeploy="true" name="localhost" unpackWARs="true"&gt;
+&lt;Valve className="org.apache.catalina.valves.AccessLogValve" directory="logs" pattern="%h %l %u %t &amp;quot;%r&amp;quot; %s %b" prefix="localhost_access_log" suffix=".txt"/&gt;
+&lt;/Host&gt;
+</t>
   </si>
   <si>
     <t>default(not use)(context.xml)
@@ -308,7 +314,7 @@
         <v>7</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C13"/>
       <c r="D13"/>
@@ -320,7 +326,7 @@
         <v>8</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C14"/>
       <c r="D14"/>

</xml_diff>